<commit_message>
FUNCTIONALITY: Moved and renamed a few keywords.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -54,9 +54,6 @@
     <t>OverlayIdentifier</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Very long run time. (~2h)</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Unwritten</t>
+  </si>
+  <si>
+    <t>Ready to Write</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,10 +613,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -628,20 +628,20 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -653,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -678,12 +678,12 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B36)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -692,33 +692,33 @@
         <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>3.0303030303030304E-2</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -727,7 +727,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: OverlayIdentifier was split into the "...Default" and "...Fields" suites. IntegrationPointKeywords - Prepping for the future.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -51,12 +51,6 @@
     <t>Percentage Automated:</t>
   </si>
   <si>
-    <t>OverlayIdentifier</t>
-  </si>
-  <si>
-    <t>Very long run time. (~2h)</t>
-  </si>
-  <si>
     <t>Writing</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>Ready to Write</t>
+  </si>
+  <si>
+    <t>OverlayIdentifierDefault</t>
+  </si>
+  <si>
+    <t>OverlayIdentifierFields</t>
   </si>
 </sst>
 </file>
@@ -179,7 +179,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -555,7 +689,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,14 +718,14 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$2:A37)</f>
+        <f>COUNTA($A$3:A38)</f>
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$2:D36,"Ready to Write")+COUNTIF($D$2:D36,"Outdated")+COUNTIF($D$2:D36,"Writing")+COUNTIF($D$2:D36,"Testing")</f>
+        <f>COUNTIF($D$3:D37,"Ready to Write")+COUNTIF($D$3:D37,"Outdated")+COUNTIF($D$3:D37,"Writing")+COUNTIF($D$3:D37,"Testing")</f>
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -604,102 +738,105 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="6">
-        <f>COUNTIF($D$2:D36,"Automated")+COUNTIF($D$2:D36,"Finished")</f>
+        <f>COUNTIF($D$3:D37,"Automated")+COUNTIF($D$3:D37,"Finished")</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
       <c r="D3" s="5" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$2:C36)</f>
-        <v>33</v>
+        <f>SUM($C$3:C37)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$2:B36)</f>
+        <f>SUM($B$3:B37)</f>
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.18181818181818182</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -707,27 +844,41 @@
         <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
         <v>0</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>13</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -745,32 +896,60 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D50">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="D3:D51">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
+      <formula>LEN(TRIM(D3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1 D3:D1048576">
+    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Step1Fields - Updated five test cases. OverlayIdentifierDefault - Continued testing. OverlayIdentifierFields - Finished testing. RDOSpecificFields - Updated the Test Case for alphabetization. Step3Fields - Updated a keyword. IntegrationPointKeywords - Fixed a keyword.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -179,7 +179,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -237,73 +237,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -689,7 +622,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +659,7 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D$3:D37,"Ready to Write")+COUNTIF($D$3:D37,"Outdated")+COUNTIF($D$3:D37,"Writing")+COUNTIF($D$3:D37,"Testing")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -757,7 +690,7 @@
       </c>
       <c r="G2" s="6">
         <f>COUNTIF($D$3:D37,"Automated")+COUNTIF($D$3:D37,"Finished")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -765,13 +698,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -818,7 +751,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$3:B37)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -836,7 +769,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.1875</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -897,58 +830,58 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D3:D51">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1 D3:D1048576">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: Updated the Test Suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -622,7 +622,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,14 +659,14 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D$3:D37,"Ready to Write")+COUNTIF($D$3:D37,"Outdated")+COUNTIF($D$3:D37,"Writing")+COUNTIF($D$3:D37,"Testing")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -763,6 +763,9 @@
       </c>
       <c r="C6" s="1">
         <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
GUI: Renamed the suites.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -72,9 +72,6 @@
     <t>WorkspaceFields</t>
   </si>
   <si>
-    <t>SourceAttributes</t>
-  </si>
-  <si>
     <t>Unwritten</t>
   </si>
   <si>
@@ -85,6 +82,15 @@
   </si>
   <si>
     <t>OverlayIdentifierFields</t>
+  </si>
+  <si>
+    <t>SourceAttributeFields</t>
+  </si>
+  <si>
+    <t>Suited to Manual</t>
+  </si>
+  <si>
+    <t>SourceAttributeLists</t>
   </si>
 </sst>
 </file>
@@ -622,7 +628,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,14 +657,14 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$3:A38)</f>
-        <v>7</v>
+        <f>COUNTA($A$3:A39)</f>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$3:D37,"Ready to Write")+COUNTIF($D$3:D37,"Outdated")+COUNTIF($D$3:D37,"Writing")+COUNTIF($D$3:D37,"Testing")</f>
+        <f>COUNTIF($D$3:D38,"Ready to Write")+COUNTIF($D$3:D38,"Outdated")+COUNTIF($D$3:D38,"Writing")+COUNTIF($D$3:D38,"Testing")</f>
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -671,7 +677,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -689,13 +695,13 @@
         <v>6</v>
       </c>
       <c r="G2" s="6">
-        <f>COUNTIF($D$3:D37,"Automated")+COUNTIF($D$3:D37,"Finished")</f>
+        <f>COUNTIF($D$3:D38,"Automated")+COUNTIF($D$3:D38,"Finished")</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -720,14 +726,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$3:C37)</f>
-        <v>32</v>
+        <f>SUM($C$3:C38)</f>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -750,7 +756,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$3:B37)</f>
+        <f>SUM($B$3:B38)</f>
         <v>12</v>
       </c>
     </row>
@@ -765,59 +771,72 @@
         <v>9</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.375</v>
+        <v>0.2608695652173913</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>5</v>
       </c>
       <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
         <v>13</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
+      <c r="D10" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -832,7 +851,7 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D3:D51">
+  <conditionalFormatting sqref="D3:D52">
     <cfRule type="notContainsBlanks" dxfId="15" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
FUNCTIONALITY: Removed outdated resource files.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -63,9 +63,6 @@
     <t>SavingErrors</t>
   </si>
   <si>
-    <t>Step3Fields</t>
-  </si>
-  <si>
     <t>WorkspaceFields</t>
   </si>
   <si>
@@ -88,6 +85,12 @@
   </si>
   <si>
     <t>SourceAttributeLists</t>
+  </si>
+  <si>
+    <t>FieldMappingsCardUI</t>
+  </si>
+  <si>
+    <t>ImportSettingsCardUI</t>
   </si>
 </sst>
 </file>
@@ -182,74 +185,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -691,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,27 +657,27 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$3:A39)</f>
-        <v>8</v>
+        <f>COUNTA($A$3:A40)</f>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$3:D38,"Ready to Write")+COUNTIF($D$3:D38,"Outdated")+COUNTIF($D$3:D38,"Writing")+COUNTIF($D$3:D38,"Testing")</f>
-        <v>3</v>
+        <f>COUNTIF($D$3:D39,"Ready to Write")+COUNTIF($D$3:D39,"Outdated")+COUNTIF($D$3:D39,"Writing")+COUNTIF($D$3:D39,"Testing")</f>
+        <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -759,13 +695,13 @@
         <v>6</v>
       </c>
       <c r="G2" s="6">
-        <f>COUNTIF($D$3:D38,"Automated")+COUNTIF($D$3:D38,"Finished")</f>
-        <v>2</v>
+        <f>COUNTIF($D$3:D39,"Automated")+COUNTIF($D$3:D39,"Finished")</f>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -784,121 +720,135 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$3:C38)</f>
-        <v>46</v>
+        <f>SUM($C$3:C39)</f>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$3:B38)</f>
-        <v>12</v>
+        <f>SUM($B$3:B39)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="1">
-        <v>9</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.2608695652173913</v>
+        <v>0.36734693877551022</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>13</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="47" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -915,31 +865,31 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D52">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D53">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: Re-wrote the Suite around two new test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -185,74 +185,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -627,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +669,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$3:C39)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -744,10 +677,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -757,7 +690,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$3:B39)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -775,7 +708,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.36734693877551022</v>
+        <v>0.39215686274509803</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -866,30 +799,30 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D2:D53">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="17" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="6" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="5" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="4" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="3" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="2" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="1" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="0" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: IntegrationPointKeywords - Wrote a few new keywords. Custodians - Re-wrote and imoproved the suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Title</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>ImportSettingsCardUI</t>
+  </si>
+  <si>
+    <t>Custodians</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Needs a Delete Keyword.</t>
   </si>
 </sst>
 </file>
@@ -185,7 +194,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -561,7 +637,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,76 +666,73 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$3:A40)</f>
-        <v>9</v>
+        <f>COUNTA($A:$A)</f>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$3:D39,"Ready to Write")+COUNTIF($D$3:D39,"Outdated")+COUNTIF($D$3:D39,"Writing")+COUNTIF($D$3:D39,"Testing")</f>
-        <v>2</v>
+        <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Writing")+COUNTIF($D:$D,"Testing")</f>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="6">
-        <f>COUNTIF($D$3:D39,"Automated")+COUNTIF($D$3:D39,"Finished")</f>
-        <v>4</v>
+        <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -668,103 +741,109 @@
         <v>8</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$3:C39)</f>
-        <v>51</v>
+        <f>SUM($C:$C)</f>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$3:B39)</f>
-        <v>20</v>
+        <f>SUM($B:$B)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.39215686274509803</v>
+        <v>0.36206896551724138</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>21</v>
@@ -772,15 +851,29 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>13</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -795,35 +888,63 @@
     <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState ref="A2:E8">
-    <sortCondition ref="A2"/>
+  <sortState ref="A2:E12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D53">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="D3:D54">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="25" stopIfTrue="1">
+      <formula>LEN(TRIM(D3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1 D3:D1048576">
+    <cfRule type="containsText" dxfId="14" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Clarified some xpaths and added a new error message to "Create Integration Point".
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Title</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>UpAndDownIcons</t>
+  </si>
+  <si>
+    <t>Long run time. (~1h:20m)</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
REFACTOR: Moved tests into a better location
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Title</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Long run time. (~1h:20m)</t>
+  </si>
+  <si>
+    <t>CustodianManagerContainsLink</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -634,7 +771,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,35 +801,35 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) - 1</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Writing")+COUNTIF($D:$D,"Testing")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -704,13 +841,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>7</v>
@@ -720,13 +857,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -736,24 +873,21 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
@@ -765,7 +899,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -777,84 +911,87 @@
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.55294117647058827</v>
+        <v>0.53409090909090906</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>20</v>
@@ -862,29 +999,43 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1">
         <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -899,62 +1050,90 @@
     <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState ref="A2:E12">
+  <sortState ref="A3:E13">
     <sortCondition ref="A2:A12"/>
   </sortState>
-  <conditionalFormatting sqref="D3:D55">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="25" stopIfTrue="1">
+  <conditionalFormatting sqref="D4:D55">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="33" stopIfTrue="1">
+      <formula>LEN(TRIM(D4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1 D4:D1048576">
+    <cfRule type="containsText" dxfId="30" priority="25" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="26" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="27" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="28" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="29" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="30" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="31" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1 D3:D1048576">
-    <cfRule type="containsText" dxfId="14" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: WIP Importnativefiles extra test for JobHistory
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Title</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>dao074</t>
+  </si>
+  <si>
+    <t>ImportNativeFiles</t>
+  </si>
+  <si>
+    <t>Ready to Write</t>
   </si>
 </sst>
 </file>
@@ -704,7 +710,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,21 +740,21 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) - 1</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Writing")+COUNTIF($D:$D,"Testing")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -806,21 +812,21 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
@@ -832,31 +838,28 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.76530612244897955</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -868,80 +871,83 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>19</v>
@@ -949,29 +955,43 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -989,12 +1009,12 @@
   <sortState ref="A3:E13">
     <sortCondition ref="A2:A12"/>
   </sortState>
-  <conditionalFormatting sqref="D4:D55">
+  <conditionalFormatting sqref="D4 D6:D55">
     <cfRule type="notContainsBlanks" dxfId="23" priority="33" stopIfTrue="1">
       <formula>LEN(TRIM(D4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1 D4:D1048576">
+  <conditionalFormatting sqref="D1 D4 D6:D1048576">
     <cfRule type="containsText" dxfId="22" priority="25" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
FUNCTIONALITY: Relocated a few test cases to a better suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -200,7 +200,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -710,7 +844,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +946,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -823,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>29</v>
@@ -833,7 +967,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -841,10 +975,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -854,7 +988,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.7142857142857143</v>
+        <v>0.74766355140186913</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1010,87 +1144,115 @@
     <sortCondition ref="A2:A12"/>
   </sortState>
   <conditionalFormatting sqref="D4 D6:D55">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="41" stopIfTrue="1">
       <formula>LEN(TRIM(D4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1 D4 D6:D1048576">
-    <cfRule type="containsText" dxfId="22" priority="25" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="38" priority="33" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="26" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="37" priority="34" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="27" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="36" priority="35" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="28" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="35" priority="36" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="29" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="34" priority="37" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="30" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="33" priority="38" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="31" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="32" priority="39" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="24" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="30" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="29" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="28" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="27" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="26" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="25" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="24" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(D5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Relocated and wrote out a few test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Title</t>
   </si>
@@ -100,12 +100,6 @@
   </si>
   <si>
     <t>dao074</t>
-  </si>
-  <si>
-    <t>ImportNativeFiles</t>
-  </si>
-  <si>
-    <t>Ready to Write</t>
   </si>
 </sst>
 </file>
@@ -200,141 +194,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -844,7 +704,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,21 +734,21 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) - 1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Writing")+COUNTIF($D:$D,"Testing")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -946,54 +806,57 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.74766355140186913</v>
+        <v>0.78703703703703709</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1005,83 +868,80 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>19</v>
@@ -1089,43 +949,29 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>16</v>
-      </c>
-      <c r="D15" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1143,116 +989,88 @@
   <sortState ref="A3:E13">
     <sortCondition ref="A2:A12"/>
   </sortState>
-  <conditionalFormatting sqref="D4 D6:D55">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="41" stopIfTrue="1">
+  <conditionalFormatting sqref="D4:D54">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="41" stopIfTrue="1">
       <formula>LEN(TRIM(D4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1 D4 D6:D1048576">
-    <cfRule type="containsText" dxfId="38" priority="33" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D1 D4:D1048576">
+    <cfRule type="containsText" dxfId="22" priority="33" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="34" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="21" priority="34" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="35" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="20" priority="35" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="36" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="19" priority="36" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="37" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="18" priority="37" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="38" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="17" priority="38" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="39" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="16" priority="39" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="24" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="24" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="30" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="14" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="13" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="10" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="6" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="5" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="4" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="3" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="2" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="1" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="0" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(D5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Updated a suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Title</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>CustodianManagerContainsLink</t>
-  </si>
-  <si>
-    <t>dao074</t>
   </si>
 </sst>
 </file>
@@ -704,7 +701,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +803,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -827,7 +824,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -851,7 +848,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.78703703703703709</v>
+        <v>0.80373831775700932</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -907,16 +904,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote two new test cases and rewrote two others.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step3/_Test_Suite_Statistics.xlsx
@@ -701,7 +701,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +803,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.80373831775700932</v>
+        <v>0.78899082568807344</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>19</v>
@@ -963,7 +963,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>7</v>

</xml_diff>